<commit_message>
Defined abstraction for cell mapping.
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/v5.xlsx
+++ b/src/test/resources/spreadsheets/v5.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="293">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -897,13 +897,31 @@
   </si>
   <si>
     <t>astrocyte</t>
+  </si>
+  <si>
+    <t>supplementary.jpg</t>
+  </si>
+  <si>
+    <t>ACS123</t>
+  </si>
+  <si>
+    <t>GEO456</t>
+  </si>
+  <si>
+    <t>AR789</t>
+  </si>
+  <si>
+    <t>INSDC001</t>
+  </si>
+  <si>
+    <t>UUID321||UUID654</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -949,6 +967,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -980,7 +1004,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -988,6 +1012,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1297,10 +1322,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1315,7 +1343,7 @@
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1363,7 +1391,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1391,9 +1419,10 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>250</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1402,9 +1431,29 @@
       <c r="C4" s="3" t="s">
         <v>248</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>292</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="59" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1527,6 +1576,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1631,6 +1681,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2232,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2475,6 +2526,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2599,6 +2651,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2606,8 +2659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2837,6 +2890,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2845,7 +2899,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3096,5 +3150,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added code to process unknown extra fields.
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/v5.xlsx
+++ b/src/test/resources/spreadsheets/v5.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="295">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -915,6 +915,12 @@
   </si>
   <si>
     <t>UUID321||UUID654</t>
+  </si>
+  <si>
+    <t>Extra field</t>
+  </si>
+  <si>
+    <t>this is a custom field</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1334,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1419,7 +1425,9 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1448,6 +1456,9 @@
       </c>
       <c r="I4" s="3" t="s">
         <v>292</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>